<commit_message>
alteração dos serviços de reprodução
</commit_message>
<xml_diff>
--- a/SAGER/presentation-app/consultarhistoricotaxaspresentation.app/server/templates/templatememoria_teifa.xlsx
+++ b/SAGER/presentation-app/consultarhistoricotaxaspresentation.app/server/templates/templatememoria_teifa.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>uge_id</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Protocolo:</t>
+  </si>
+  <si>
+    <t>duracao</t>
+  </si>
+  <si>
+    <t>tpparametro</t>
   </si>
 </sst>
 </file>
@@ -215,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -224,12 +230,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5154"/>
+  <dimension ref="A1:T5154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5131" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,60 +639,60 @@
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="L8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -737,27 +744,33 @@
       <c r="R9" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -30497,16 +30510,16 @@
       <c r="D5153" s="7"/>
     </row>
     <row r="5154" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5154" s="9"/>
-      <c r="B5154" s="10"/>
-      <c r="C5154" s="10"/>
-      <c r="D5154" s="10"/>
-      <c r="E5154" s="11"/>
-      <c r="F5154" s="11"/>
-      <c r="G5154" s="11"/>
-      <c r="H5154" s="11"/>
-      <c r="I5154" s="11"/>
-      <c r="J5154" s="11"/>
+      <c r="A5154" s="8"/>
+      <c r="B5154" s="9"/>
+      <c r="C5154" s="9"/>
+      <c r="D5154" s="9"/>
+      <c r="E5154" s="10"/>
+      <c r="F5154" s="10"/>
+      <c r="G5154" s="10"/>
+      <c r="H5154" s="10"/>
+      <c r="I5154" s="10"/>
+      <c r="J5154" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
melhorias para apresentação das retificações
</commit_message>
<xml_diff>
--- a/SAGER/presentation-app/consultarhistoricotaxaspresentation.app/server/templates/templatememoria_teifa.xlsx
+++ b/SAGER/presentation-app/consultarhistoricotaxaspresentation.app/server/templates/templatememoria_teifa.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>uge_id</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Iníco Oper</t>
   </si>
   <si>
-    <t>desger_id</t>
-  </si>
-  <si>
     <t>Protocolo:</t>
   </si>
   <si>
@@ -103,6 +100,12 @@
   </si>
   <si>
     <t>tpparametro</t>
+  </si>
+  <si>
+    <t>versao</t>
+  </si>
+  <si>
+    <t>numons</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -619,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T5154"/>
+  <dimension ref="A1:U5154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,43 +642,43 @@
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
@@ -692,7 +695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -724,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>0</v>
@@ -745,32 +748,35 @@
         <v>5</v>
       </c>
       <c r="S9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="11" t="s">
+      <c r="U9" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>